<commit_message>
Consertou tratamento da data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -975,13 +975,13 @@
         </is>
       </c>
       <c r="B34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -991,13 +991,13 @@
         </is>
       </c>
       <c r="B35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>